<commit_message>
kinetic new init guesses
</commit_message>
<xml_diff>
--- a/supplementary/data5/kinetic.xlsx
+++ b/supplementary/data5/kinetic.xlsx
@@ -1236,13 +1236,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.088868784456559</v>
+        <v>7.091375396763511</v>
       </c>
       <c r="C2" t="n">
-        <v>7.085903931617888</v>
+        <v>7.08834646822768</v>
       </c>
       <c r="D2" t="n">
-        <v>7.09173918651934</v>
+        <v>7.094588348398556</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1255,13 +1255,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2218042731260738</v>
+        <v>0.2155541022706274</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2172569335315839</v>
+        <v>0.2111825662029117</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2259443603163205</v>
+        <v>0.2194174109286831</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1274,13 +1274,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9627777866885804</v>
+        <v>0.9850318872564032</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9582893998925268</v>
+        <v>0.9808335656417604</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9665462154654424</v>
+        <v>0.9890955125464962</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -1293,13 +1293,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04299816868683828</v>
+        <v>0.04570409132987917</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0416581880208682</v>
+        <v>0.044466523144024</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0443362877270005</v>
+        <v>0.0471422109644458</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -1310,13 +1310,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04490516687120605</v>
+        <v>0.04796223935454592</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0434690292369121</v>
+        <v>0.0465358088792204</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0463931907398113</v>
+        <v>0.0494745507187214</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.841828933920632</v>
+        <v>3.977194255830469</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8746754394370072</v>
+        <v>0.9213745868170952</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8763620191238604</v>
+        <v>0.9659773182121414</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1368,7 +1368,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8842270585595692</v>
+        <v>0.8858075040783034</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1381,7 +1381,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>94987</v>
+        <v>94943</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1394,7 +1394,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>516</v>
+        <v>560</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>556</v>
+        <v>153</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3941</v>
+        <v>4344</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -1433,13 +1433,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9413151492552663</v>
+        <v>0.9498755236272217</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7433924432155734</v>
+        <v>0.8741499762503702</v>
       </c>
       <c r="D15" t="n">
-        <v>0.973606631246742</v>
+        <v>0.9732550492492644</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -1450,13 +1450,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01847270131111145</v>
+        <v>0.01770749874413013</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01813729107379913</v>
+        <v>0.01736527681350708</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01879766210913658</v>
+        <v>0.01804036274552345</v>
       </c>
       <c r="E16" t="n">
         <v>0.01</v>
@@ -1469,13 +1469,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.4250694513320923</v>
+        <v>0.3674274384975433</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4170733690261841</v>
+        <v>0.3593991994857788</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4331128597259521</v>
+        <v>0.3752899765968323</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -1529,13 +1529,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.031250575260395</v>
+        <v>7.06021125524706</v>
       </c>
       <c r="C2" t="n">
-        <v>7.028514947141549</v>
+        <v>7.056842005000705</v>
       </c>
       <c r="D2" t="n">
-        <v>7.033899019368281</v>
+        <v>7.063785299880137</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1548,13 +1548,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2162943215754058</v>
+        <v>0.2130378687845743</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2137450208698239</v>
+        <v>0.2104350710880794</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2186018993193142</v>
+        <v>0.2153324042271456</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1567,13 +1567,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1500529229281627</v>
+        <v>0.1489274750971695</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1482304049400499</v>
+        <v>0.1472309718352218</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1515882710773636</v>
+        <v>0.1505752564049686</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -1586,13 +1586,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08321811710647099</v>
+        <v>0.09146597914583891</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08168085477347189</v>
+        <v>0.08975361143246929</v>
       </c>
       <c r="D5" t="n">
-        <v>0.08476461982538259</v>
+        <v>0.0934870118728892</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -1603,13 +1603,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09073987026349598</v>
+        <v>0.1007820415000232</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0889460436587718</v>
+        <v>0.0986036458254857</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0926151039192733</v>
+        <v>0.1031281556454447</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.780630810192404</v>
+        <v>3.794913657127249</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9777715468389998</v>
+        <v>0.9869668033489287</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1648,7 +1648,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.979381443298969</v>
+        <v>0.9971883786316776</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9799554565701559</v>
+        <v>0.9790660225442834</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1674,7 +1674,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>91293</v>
+        <v>91282</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>176</v>
+        <v>24</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>8360</v>
+        <v>8512</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -1726,13 +1726,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9952905979097751</v>
+        <v>0.9959912955627339</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9885638197039148</v>
+        <v>0.990893437813048</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9968279805170086</v>
+        <v>0.9972758696812904</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -1743,13 +1743,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02321786992251873</v>
+        <v>0.02295475080609322</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02294084802269936</v>
+        <v>0.02267354354262352</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02348874136805534</v>
+        <v>0.02327138930559158</v>
       </c>
       <c r="E16" t="n">
         <v>0.02</v>
@@ -1762,13 +1762,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2487180531024933</v>
+        <v>0.2389774024486542</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2459967881441116</v>
+        <v>0.2363721132278442</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2514059245586395</v>
+        <v>0.2419286072254181</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -1822,13 +1822,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.04065727277566</v>
+        <v>7.026457620318788</v>
       </c>
       <c r="C2" t="n">
-        <v>7.037541065032656</v>
+        <v>7.023006260804793</v>
       </c>
       <c r="D2" t="n">
-        <v>7.043674241926231</v>
+        <v>7.030118792250823</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1841,13 +1841,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2156395975687813</v>
+        <v>0.2084545695551597</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2132791468871897</v>
+        <v>0.2062346187324851</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2177749632184782</v>
+        <v>0.2104091263551493</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1860,13 +1860,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01001474248746577</v>
+        <v>0.01011495651878666</v>
       </c>
       <c r="C4" t="n">
-        <v>0.009537832206037799</v>
+        <v>0.0096873542259288</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0104230609315133</v>
+        <v>0.01053663073053</v>
       </c>
       <c r="E4" t="n">
         <v>0.01</v>
@@ -1879,13 +1879,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08550665725691407</v>
+        <v>0.08842102395588299</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08393572779296241</v>
+        <v>0.0866312029481302</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0870890978602484</v>
+        <v>0.0905366464865939</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -1896,13 +1896,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09346864248481367</v>
+        <v>0.09710949610326858</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0916264615824165</v>
+        <v>0.0948479999473003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0953971495691788</v>
+        <v>0.0995495278421783</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.748669710010494</v>
+        <v>3.754995153400072</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -1928,7 +1928,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.997568245245115</v>
+        <v>0.9982102806303779</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1941,7 +1941,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9984770384254921</v>
+        <v>0.9997656982193065</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9970753392606457</v>
+        <v>0.9969626168224299</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>91439</v>
+        <v>91438</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1980,7 +1980,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1993,7 +1993,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -2006,7 +2006,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>8523</v>
+        <v>8534</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -2019,13 +2019,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.999706631796323</v>
+        <v>0.9997163097722556</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9993523465424894</v>
+        <v>0.9993532012719424</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9997947893615488</v>
+        <v>0.9998065850724148</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -2036,13 +2036,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02074295468628407</v>
+        <v>0.02143225818872452</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02050240710377693</v>
+        <v>0.0211155116558075</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02097185887396336</v>
+        <v>0.02174844592809677</v>
       </c>
       <c r="E16" t="n">
         <v>0.02</v>
@@ -2055,13 +2055,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2186738401651382</v>
+        <v>0.2236988991498947</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2166740000247955</v>
+        <v>0.2211383283138275</v>
       </c>
       <c r="D17" t="n">
-        <v>0.220608651638031</v>
+        <v>0.2262476980686188</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -2115,13 +2115,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.066881681521902</v>
+        <v>7.069538363303134</v>
       </c>
       <c r="C2" t="n">
-        <v>7.06374987417586</v>
+        <v>7.066471547198036</v>
       </c>
       <c r="D2" t="n">
-        <v>7.069913754280773</v>
+        <v>7.072791515900962</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2134,13 +2134,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2178240155347146</v>
+        <v>0.2140253691895748</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2147797317860449</v>
+        <v>0.211112084360276</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2205837719392568</v>
+        <v>0.2165941194259719</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -2153,13 +2153,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4925623015000863</v>
+        <v>0.4942537415083439</v>
       </c>
       <c r="C4" t="n">
-        <v>0.489531690178382</v>
+        <v>0.491348637547241</v>
       </c>
       <c r="D4" t="n">
-        <v>0.495108496379895</v>
+        <v>0.4970678487643808</v>
       </c>
       <c r="E4" t="n">
         <v>0.5</v>
@@ -2172,13 +2172,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08270107106940353</v>
+        <v>0.08794474705158052</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0811976376363323</v>
+        <v>0.08641583659590139</v>
       </c>
       <c r="D5" t="n">
-        <v>0.084212570873285</v>
+        <v>0.0897499983595077</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -2189,13 +2189,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09012578318659099</v>
+        <v>0.0965200382973623</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08837334444052709</v>
+        <v>0.0945899026210584</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0919564608692873</v>
+        <v>0.0985992847283918</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -2206,7 +2206,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.807196334102034</v>
+        <v>3.888352786270419</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -2221,7 +2221,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9385588463194752</v>
+        <v>0.9673485997409966</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -2234,7 +2234,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9334582942830365</v>
+        <v>0.9886363636363636</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9541372290743624</v>
+        <v>0.9520532490974729</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -2260,7 +2260,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>91081</v>
+        <v>91039</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2273,7 +2273,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>383</v>
+        <v>425</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -2286,7 +2286,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>568</v>
+        <v>97</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -2299,7 +2299,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7968</v>
+        <v>8439</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -2312,13 +2312,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.983895780166482</v>
+        <v>0.9863422355680398</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9503344467290578</v>
+        <v>0.9683463279073644</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9921699022251912</v>
+        <v>0.9932185867265756</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -2329,13 +2329,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02767674811184406</v>
+        <v>0.02600592747330666</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02738365158438683</v>
+        <v>0.02566586062312126</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02797280810773373</v>
+        <v>0.02634398639202118</v>
       </c>
       <c r="E16" t="n">
         <v>0.02</v>
@@ -2348,13 +2348,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3096111118793488</v>
+        <v>0.2714546620845795</v>
       </c>
       <c r="C17" t="n">
-        <v>0.306219220161438</v>
+        <v>0.2677920460700989</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3131935000419617</v>
+        <v>0.2750931978225708</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -2674,13 +2674,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.100768899757334</v>
+        <v>7.09360828376252</v>
       </c>
       <c r="C2" t="n">
-        <v>7.097723466341554</v>
+        <v>7.090574075573116</v>
       </c>
       <c r="D2" t="n">
-        <v>7.103717329822871</v>
+        <v>7.096826836858833</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2230786789385459</v>
+        <v>0.2153095270542503</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2198648068537557</v>
+        <v>0.2122213534336023</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2259971037251177</v>
+        <v>0.2180318906830289</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -2712,13 +2712,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9605101748297807</v>
+        <v>0.9781940071850105</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9558978128454814</v>
+        <v>0.973980966120743</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9643829366297562</v>
+        <v>0.9822719685112939</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -2731,13 +2731,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.07661475153698845</v>
+        <v>0.08768762340848346</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0748277311646782</v>
+        <v>0.0861530183928151</v>
       </c>
       <c r="D5" t="n">
-        <v>0.07841001815863009</v>
+        <v>0.0894998189440655</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -2748,13 +2748,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.082935018578909</v>
+        <v>0.09621131944302815</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0808797817428204</v>
+        <v>0.0942751035574533</v>
       </c>
       <c r="D6" t="n">
-        <v>0.085081239713236</v>
+        <v>0.09829742108044209</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.84891868091762</v>
+        <v>3.976332533586507</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -2780,7 +2780,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9016014291771309</v>
+        <v>0.9475752096002545</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -2793,7 +2793,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8914011246485474</v>
+        <v>0.9783270852858482</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2806,7 +2806,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9286062972907005</v>
+        <v>0.926653351087439</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -2819,7 +2819,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>90879</v>
+        <v>90803</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>585</v>
+        <v>661</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -2845,7 +2845,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>927</v>
+        <v>185</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -2858,7 +2858,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7609</v>
+        <v>8351</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -2871,13 +2871,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9663999110452866</v>
+        <v>0.9748970424226151</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8657653787352899</v>
+        <v>0.9393870715638608</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9847034071472012</v>
+        <v>0.986780418531541</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -2888,13 +2888,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0316612720489502</v>
+        <v>0.02919815294444561</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03128522261977196</v>
+        <v>0.02882345393300056</v>
       </c>
       <c r="D16" t="n">
-        <v>0.03201822936534882</v>
+        <v>0.02959552407264709</v>
       </c>
       <c r="E16" t="n">
         <v>0.02</v>
@@ -2907,13 +2907,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3702596426010132</v>
+        <v>0.3055579364299774</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3649614751338959</v>
+        <v>0.3011916875839233</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3752395510673523</v>
+        <v>0.3100284934043884</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -2967,13 +2967,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.104133528249515</v>
+        <v>7.11231498831246</v>
       </c>
       <c r="C2" t="n">
-        <v>7.101085724869591</v>
+        <v>7.109027234294032</v>
       </c>
       <c r="D2" t="n">
-        <v>7.107084252968354</v>
+        <v>7.115802555429863</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2986,13 +2986,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2241267408474479</v>
+        <v>0.2135277204321303</v>
       </c>
       <c r="C3" t="n">
-        <v>0.221532752191715</v>
+        <v>0.2112009890877539</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2264797218047128</v>
+        <v>0.2155772853691782</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -3005,13 +3005,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9593973041988441</v>
+        <v>0.9760516754645083</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9547638681534176</v>
+        <v>0.971587234815104</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9632878089915016</v>
+        <v>0.980373536587786</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -3024,13 +3024,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1162261925747684</v>
+        <v>0.1339251735108984</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1142474080488491</v>
+        <v>0.1317617859596624</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1182112438540393</v>
+        <v>0.1363456143985662</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -3041,13 +3041,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1314674060559528</v>
+        <v>0.1547796573484601</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1289834307023066</v>
+        <v>0.1517576457322563</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1340584616884752</v>
+        <v>0.1578705749367354</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -3058,7 +3058,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.857695339193204</v>
+        <v>3.973909885425272</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -3073,7 +3073,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9129423005269492</v>
+        <v>0.96076456904789</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -3086,7 +3086,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9012432559230589</v>
+        <v>0.9859254046446164</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -3099,7 +3099,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9468495851474575</v>
+        <v>0.9461954074741108</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>86564</v>
+        <v>86494</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -3125,7 +3125,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>647</v>
+        <v>717</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -3138,7 +3138,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1263</v>
+        <v>180</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -3151,7 +3151,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11526</v>
+        <v>12609</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -3164,13 +3164,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9787722537815802</v>
+        <v>0.9843029989683195</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9182121581630044</v>
+        <v>0.9630866457314344</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9905784793420626</v>
+        <v>0.991780098910147</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -3181,13 +3181,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.04513679817318916</v>
+        <v>0.04102649167180061</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04475420713424683</v>
+        <v>0.04059755057096481</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04556970298290253</v>
+        <v>0.04149503260850906</v>
       </c>
       <c r="E16" t="n">
         <v>0.03</v>
@@ -3200,13 +3200,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.335505485534668</v>
+        <v>0.2730682492256165</v>
       </c>
       <c r="C17" t="n">
-        <v>0.332321435213089</v>
+        <v>0.2699359059333801</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3386399745941162</v>
+        <v>0.2762128710746765</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -3260,13 +3260,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.028840212650846</v>
+        <v>7.04628794938082</v>
       </c>
       <c r="C2" t="n">
-        <v>7.025993309933431</v>
+        <v>7.043125529701958</v>
       </c>
       <c r="D2" t="n">
-        <v>7.031596405330973</v>
+        <v>7.049642541020615</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -3279,13 +3279,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2174347088879093</v>
+        <v>0.2135157273658656</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2138186250755662</v>
+        <v>0.210010275324963</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2207166920576225</v>
+        <v>0.216611060200277</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -3298,13 +3298,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1513944739947845</v>
+        <v>0.1505743735536307</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1496470326118017</v>
+        <v>0.1489205773381682</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1528661740243312</v>
+        <v>0.1521803546675125</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -3317,13 +3317,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04329161348648818</v>
+        <v>0.04632437690086312</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0421589328399918</v>
+        <v>0.0452062373083401</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0444206308215615</v>
+        <v>0.0476222563694147</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -3334,13 +3334,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0452294530963893</v>
+        <v>0.04863715045225923</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0440145389898733</v>
+        <v>0.0473465989691828</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0464855490503641</v>
+        <v>0.0500035377047646</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -3351,7 +3351,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.777942180358695</v>
+        <v>3.799857406727484</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -3366,7 +3366,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9712528782947377</v>
+        <v>0.9804755263655053</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -3379,7 +3379,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9766511007338226</v>
+        <v>0.9955525906159662</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9684674751929437</v>
+        <v>0.9673725151253241</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -3405,7 +3405,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>95360</v>
+        <v>95352</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -3418,7 +3418,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -3431,7 +3431,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -3444,7 +3444,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4392</v>
+        <v>4477</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -3457,13 +3457,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9905309366232037</v>
+        <v>0.991553947980085</v>
       </c>
       <c r="C15" t="n">
-        <v>0.977141216720351</v>
+        <v>0.981190323262744</v>
       </c>
       <c r="D15" t="n">
-        <v>0.99353129393828</v>
+        <v>0.9942547691912016</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -3474,13 +3474,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01245281845331192</v>
+        <v>0.01229405216872692</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01222751475870609</v>
+        <v>0.01205978915095329</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01265196222811937</v>
+        <v>0.01254850812256336</v>
       </c>
       <c r="E16" t="n">
         <v>0.01</v>
@@ -3493,13 +3493,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2641052603721619</v>
+        <v>0.2536819875240326</v>
       </c>
       <c r="C17" t="n">
-        <v>0.259624183177948</v>
+        <v>0.248997837305069</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2681658267974854</v>
+        <v>0.2583458423614502</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -3553,13 +3553,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.034446788084989</v>
+        <v>7.035305914076499</v>
       </c>
       <c r="C2" t="n">
-        <v>7.031739765444332</v>
+        <v>7.031796552736279</v>
       </c>
       <c r="D2" t="n">
-        <v>7.037067533241993</v>
+        <v>7.03902862890179</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -3572,13 +3572,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2089481455079836</v>
+        <v>0.2053589974979707</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2055163826310234</v>
+        <v>0.2023127758440727</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2120549476124516</v>
+        <v>0.2080444701786377</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -3591,13 +3591,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.009794016569154801</v>
+        <v>0.009941386396188615</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0093510829226187</v>
+        <v>0.009501954003986301</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0101728270262937</v>
+        <v>0.0103751411091958</v>
       </c>
       <c r="E4" t="n">
         <v>0.01</v>
@@ -3610,13 +3610,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04511294827584469</v>
+        <v>0.0461384226180436</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0440559192891341</v>
+        <v>0.044996721260403</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0461672057856651</v>
+        <v>0.0474639016490159</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -3627,13 +3627,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04722440863068247</v>
+        <v>0.04843403595983169</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0460862934376221</v>
+        <v>0.0471168239345442</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0484017814403982</v>
+        <v>0.049828979473516</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -3644,7 +3644,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.753469173143859</v>
+        <v>3.757432758144986</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -3659,7 +3659,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9975580414740786</v>
+        <v>0.9979096996982701</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9986657771847899</v>
+        <v>0.9997776295307983</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -3685,7 +3685,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9966711051930759</v>
+        <v>0.9962331043651673</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -3698,7 +3698,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>95488</v>
+        <v>95486</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -3711,7 +3711,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -3724,7 +3724,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -3737,7 +3737,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4491</v>
+        <v>4496</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -3750,13 +3750,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9994542050243885</v>
+        <v>0.9994597468346466</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9987234739327442</v>
+        <v>0.9987079121676512</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9996194486795018</v>
+        <v>0.99962921658922</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -3767,13 +3767,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01050676684826612</v>
+        <v>0.01083271391689777</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01035144552588463</v>
+        <v>0.01060754433274269</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01071084477007389</v>
+        <v>0.01105181407183409</v>
       </c>
       <c r="E16" t="n">
         <v>0.01</v>
@@ -3786,13 +3786,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2198658138513565</v>
+        <v>0.2247177362442017</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2172080278396606</v>
+        <v>0.2211559414863586</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2233273684978485</v>
+        <v>0.2282173037528992</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -3846,13 +3846,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.060522531993679</v>
+        <v>7.076247558832254</v>
       </c>
       <c r="C2" t="n">
-        <v>7.057660559784917</v>
+        <v>7.073072826643915</v>
       </c>
       <c r="D2" t="n">
-        <v>7.063293314414879</v>
+        <v>7.079615210894249</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -3865,13 +3865,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2205099251683135</v>
+        <v>0.2119838761813904</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2181193877374279</v>
+        <v>0.2098091677298893</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2226753876450748</v>
+        <v>0.2139001913975675</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -3884,13 +3884,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4932072806784642</v>
+        <v>0.4930559391925696</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4902270562004052</v>
+        <v>0.4899298333790815</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4957110183852504</v>
+        <v>0.4960848069756262</v>
       </c>
       <c r="E4" t="n">
         <v>0.5</v>
@@ -3903,13 +3903,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1237091945397786</v>
+        <v>0.1302463729734762</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1218243608822544</v>
+        <v>0.1282790263999227</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1256083489608222</v>
+        <v>0.1324535928373539</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -3920,13 +3920,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.141130980182585</v>
+        <v>0.1498819418745603</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1387243684094533</v>
+        <v>0.1471560643515574</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1436522743624303</v>
+        <v>0.1526760894366334</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.818784980518349</v>
+        <v>3.887477549947963</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -3952,7 +3952,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.946611530641954</v>
+        <v>0.975598354588578</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -3965,7 +3965,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9407303151145515</v>
+        <v>0.9928063179294706</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -3978,7 +3978,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9661125833132579</v>
+        <v>0.9648909491602705</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -3991,7 +3991,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>86789</v>
+        <v>86749</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -4004,7 +4004,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>422</v>
+        <v>462</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -4017,7 +4017,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>758</v>
+        <v>92</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -4030,7 +4030,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12031</v>
+        <v>12697</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -4043,13 +4043,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9896296221543096</v>
+        <v>0.9911685809094287</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9695267699393272</v>
+        <v>0.979884172984994</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9948916384909297</v>
+        <v>0.9953544553447315</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -4060,13 +4060,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.04034782573580742</v>
+        <v>0.03766826540231705</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03995432332158089</v>
+        <v>0.03732733055949211</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04070852696895599</v>
+        <v>0.03807415813207626</v>
       </c>
       <c r="E16" t="n">
         <v>0.03</v>
@@ -4079,13 +4079,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2866074740886688</v>
+        <v>0.2502128183841705</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2839456796646118</v>
+        <v>0.247850626707077</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2893470525741577</v>
+        <v>0.2527241408824921</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -4139,13 +4139,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.05034144635217</v>
+        <v>7.042549519834179</v>
       </c>
       <c r="C2" t="n">
-        <v>7.047639709813579</v>
+        <v>7.039401660051236</v>
       </c>
       <c r="D2" t="n">
-        <v>7.052957071934907</v>
+        <v>7.045888663570635</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -4158,13 +4158,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2161340907351461</v>
+        <v>0.2137511836636766</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2139814034928323</v>
+        <v>0.2117384111642842</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2180808484736656</v>
+        <v>0.2155228820471171</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -4177,13 +4177,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1507820779584677</v>
+        <v>0.1487924711592156</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1489394432458142</v>
+        <v>0.1471205961935708</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1523344254487793</v>
+        <v>0.1504162086118642</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -4196,13 +4196,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1296271650524902</v>
+        <v>0.1283574568669582</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1276707029937006</v>
+        <v>0.1264398857449973</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1316038545417808</v>
+        <v>0.130512381206068</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -4213,13 +4213,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.148887968321898</v>
+        <v>0.1473866796083394</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1463560875835381</v>
+        <v>0.1447409113590815</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1515481796504766</v>
+        <v>0.1501026333274808</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -4230,7 +4230,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.775438067256976</v>
+        <v>3.799344570908354</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -4245,7 +4245,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9815432611825936</v>
+        <v>0.9902721670349944</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -4258,7 +4258,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9817030260380014</v>
+        <v>0.9984361560716241</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -4271,7 +4271,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9860980207351555</v>
+        <v>0.9846545342381247</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -4284,7 +4284,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>87034</v>
+        <v>87012</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -4297,7 +4297,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -4310,7 +4310,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>234</v>
+        <v>20</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -4323,7 +4323,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12555</v>
+        <v>12769</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -4336,13 +4336,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9971131654898711</v>
+        <v>0.9972715362139604</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9930999209205954</v>
+        <v>0.9938698930218396</v>
       </c>
       <c r="D15" t="n">
-        <v>0.998026576493002</v>
+        <v>0.9981132131350404</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -4353,13 +4353,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0346968024969101</v>
+        <v>0.03437121585011482</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03431495651602745</v>
+        <v>0.0340239480137825</v>
       </c>
       <c r="D16" t="n">
-        <v>0.03506641834974289</v>
+        <v>0.03472421318292618</v>
       </c>
       <c r="E16" t="n">
         <v>0.03</v>
@@ -4372,13 +4372,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2363456189632416</v>
+        <v>0.2279951125383377</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2341872155666351</v>
+        <v>0.2260666787624359</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2385842800140381</v>
+        <v>0.2299944162368774</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -4432,13 +4432,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.050076890305859</v>
+        <v>7.07724249945597</v>
       </c>
       <c r="C2" t="n">
-        <v>7.047068382419779</v>
+        <v>7.074058997340966</v>
       </c>
       <c r="D2" t="n">
-        <v>7.052989568105279</v>
+        <v>7.080619456476558</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -4451,13 +4451,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2193267452248493</v>
+        <v>0.2145375543957383</v>
       </c>
       <c r="C3" t="n">
-        <v>0.215132179183123</v>
+        <v>0.2104263003518859</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2231404295644541</v>
+        <v>0.2181706140906058</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -4470,13 +4470,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4960500045688493</v>
+        <v>0.5026349434874411</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4930179682995274</v>
+        <v>0.4995867513067848</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4985973503154896</v>
+        <v>0.5055879250171001</v>
       </c>
       <c r="E4" t="n">
         <v>0.5</v>
@@ -4489,13 +4489,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04118987766080785</v>
+        <v>0.04608334465703535</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0400123256002055</v>
+        <v>0.0448315933013751</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0423623930394758</v>
+        <v>0.0475384278644474</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -4506,13 +4506,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.04293757916677422</v>
+        <v>0.04837971824790553</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0416800411656653</v>
+        <v>0.0469358001045122</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0442363517316988</v>
+        <v>0.0499111242995269</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -4523,7 +4523,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.803402403095717</v>
+        <v>3.880147389405924</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -4538,7 +4538,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9218993009940205</v>
+        <v>0.9493524961084389</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -4551,7 +4551,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9270624861018457</v>
+        <v>0.9833222148098733</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -4564,7 +4564,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9237757589186794</v>
+        <v>0.9210581128931472</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -4577,7 +4577,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>95159</v>
+        <v>95124</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -4590,7 +4590,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>344</v>
+        <v>379</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -4603,7 +4603,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>328</v>
+        <v>75</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -4616,7 +4616,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4169</v>
+        <v>4422</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -4629,13 +4629,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9662574667501803</v>
+        <v>0.9726351096474413</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8929221143725041</v>
+        <v>0.9343703467691786</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9819799823867232</v>
+        <v>0.9857412069469136</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -4646,13 +4646,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01579182781279087</v>
+        <v>0.01510802283883095</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01552303694188595</v>
+        <v>0.014832878485322</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01606413535773754</v>
+        <v>0.01542406342923641</v>
       </c>
       <c r="E16" t="n">
         <v>0.01</v>
@@ -4665,13 +4665,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3500876128673553</v>
+        <v>0.311340868473053</v>
       </c>
       <c r="C17" t="n">
-        <v>0.343183159828186</v>
+        <v>0.3050098419189453</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3564581871032715</v>
+        <v>0.3182963132858276</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>
@@ -4725,13 +4725,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.03508365681678</v>
+        <v>7.046951384465913</v>
       </c>
       <c r="C2" t="n">
-        <v>7.032416584353249</v>
+        <v>7.043795596104342</v>
       </c>
       <c r="D2" t="n">
-        <v>7.037665718279488</v>
+        <v>7.050298940074221</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -4744,13 +4744,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2117008052897014</v>
+        <v>0.2105536799174863</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2097640816501526</v>
+        <v>0.2085003492658259</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2134493472842259</v>
+        <v>0.2123618010587373</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -4763,13 +4763,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.00974777710136801</v>
+        <v>0.009995406382794121</v>
       </c>
       <c r="C4" t="n">
-        <v>0.009306870745006799</v>
+        <v>0.0095522160963532</v>
       </c>
       <c r="D4" t="n">
-        <v>0.010124854894641</v>
+        <v>0.0104329001812614</v>
       </c>
       <c r="E4" t="n">
         <v>0.01</v>
@@ -4782,13 +4782,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1318137783755936</v>
+        <v>0.128484297407675</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1297728630976562</v>
+        <v>0.1264397821520622</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1338763725796654</v>
+        <v>0.1307828435853041</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -4799,13 +4799,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1517795700387295</v>
+        <v>0.1475622447236769</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1491252773109014</v>
+        <v>0.1447407758096166</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1545695890802791</v>
+        <v>0.1504604949894885</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -4816,7 +4816,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.748835517913848</v>
+        <v>3.746266141658285</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -4831,7 +4831,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9977152900690317</v>
+        <v>0.998165367415366</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -4844,7 +4844,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9986707326608805</v>
+        <v>0.9997654234107436</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -4857,7 +4857,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9973449945338123</v>
+        <v>0.9970368059887711</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -4870,7 +4870,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>87177</v>
+        <v>87173</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -4883,7 +4883,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -4896,7 +4896,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
@@ -4909,7 +4909,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12772</v>
+        <v>12786</v>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
@@ -4922,13 +4922,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9998257440880964</v>
+        <v>0.9998142693871795</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9995946434406136</v>
+        <v>0.9995750015233966</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9998811821222851</v>
+        <v>0.9998730391805511</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -4939,13 +4939,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.03202880546450615</v>
+        <v>0.03284154459834099</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03174693882465363</v>
+        <v>0.03245498239994049</v>
       </c>
       <c r="D16" t="n">
-        <v>0.03235426545143127</v>
+        <v>0.03320459276437759</v>
       </c>
       <c r="E16" t="n">
         <v>0.03</v>
@@ -4958,13 +4958,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2145080268383026</v>
+        <v>0.2181949317455292</v>
       </c>
       <c r="C17" t="n">
-        <v>0.213030070066452</v>
+        <v>0.2161856889724731</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2162074446678162</v>
+        <v>0.2200497388839722</v>
       </c>
       <c r="E17" t="n">
         <v>0.2</v>

</xml_diff>